<commit_message>
chore (Tests): pequenas modificações nos arquivos de dados usados para teste das funções.
</commit_message>
<xml_diff>
--- a/tests/testthat/dataForTests/DP.SCA2.xlsx
+++ b/tests/testthat/dataForTests/DP.SCA2.xlsx
@@ -1,35 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f255b83a8ca26df5/Documentos/TestesBLUPF90/XLSX/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26844A69-5132-48D8-9029-348816375676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C8BD22F0-19C2-4346-B3BD-36540F82936D}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -38,41 +22,59 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Ordem</t>
+    <t xml:space="preserve">Ordem</t>
   </si>
   <si>
     <t xml:space="preserve">Lote </t>
   </si>
   <si>
-    <t>N°</t>
+    <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t>DataCast</t>
+    <t xml:space="preserve">DataCast</t>
   </si>
   <si>
-    <t>GanhoM1</t>
+    <t xml:space="preserve">GanhoM1</t>
   </si>
   <si>
-    <t>UltimaP</t>
+    <t xml:space="preserve">UltimaP</t>
   </si>
   <si>
-    <t>GanhoM2</t>
+    <t xml:space="preserve">GanhoM2</t>
   </si>
   <si>
-    <t>Peso</t>
+    <t xml:space="preserve">Peso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,7 +86,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -92,218 +94,140 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="0e2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="e8e8e8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="e97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="196b24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="0f9ed5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="a02b93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="4ea72e"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="96607d"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -311,33 +235,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -350,13 +265,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -366,15 +275,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -382,7 +289,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -390,800 +296,787 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3473016E-298B-45DE-9139-B52ADE9C272F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.13"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0" t="n">
         <v>0.89</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>433</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0" t="n">
         <v>0.48</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0" t="n">
         <v>460</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0" t="n">
         <v>330</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0" t="n">
         <v>1.49</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0" t="n">
         <v>443</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0" t="n">
         <v>-0.63</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0" t="n">
         <v>408</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0" t="n">
         <v>89</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0" t="n">
         <v>356</v>
       </c>
-      <c r="E4">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="0" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>443</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0" t="n">
         <v>0.36</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0" t="n">
         <v>463</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0" t="n">
         <v>203</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0" t="n">
         <v>360</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0" t="n">
         <v>1.04</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0" t="n">
         <v>439</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0" t="n">
         <v>0.52</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0" t="n">
         <v>468</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0" t="n">
         <v>209</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0" t="n">
         <v>352</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0" t="n">
         <v>1.22</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0" t="n">
         <v>445</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0" t="n">
         <v>0.36</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0" t="n">
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0" t="n">
         <v>674</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0" t="n">
         <v>355</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0" t="n">
         <v>1.08</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0" t="n">
         <v>437</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0" t="n">
         <v>0.43</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0" t="n">
         <v>461</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0" t="n">
         <v>696</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0" t="n">
         <v>1.08</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0" t="n">
         <v>447</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0" t="n">
         <v>0.38</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0" t="n">
         <v>468</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0" t="n">
         <v>701</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0" t="n">
         <v>363</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0" t="n">
         <v>1.03</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0" t="n">
         <v>441</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0" t="n">
         <v>0.48</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="0" t="n">
         <v>468</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0" t="n">
         <v>710</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0" t="n">
         <v>369</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="0" t="n">
         <v>0.89</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0" t="n">
         <v>437</v>
       </c>
-      <c r="G10">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="0" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0" t="n">
         <v>738</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="0" t="n">
         <v>336</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="0" t="n">
         <v>1.07</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0" t="n">
         <v>417</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="0" t="n">
         <v>0.41</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="0" t="n">
         <v>440</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="0" t="n">
         <v>362</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="0" t="n">
         <v>0.8</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0" t="n">
         <v>421</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="0" t="n">
         <v>449</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="0" t="n">
         <v>245</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="0" t="n">
         <v>372</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="0" t="n">
         <v>0.64</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0" t="n">
         <v>419</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="0" t="n">
         <v>0.32</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0" t="n">
         <v>437</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0" t="n">
         <v>669</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="0" t="n">
         <v>367</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="0" t="n">
         <v>0.74</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0" t="n">
         <v>422</v>
       </c>
-      <c r="G14">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H14">
+      <c r="G14" s="0" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H14" s="0" t="n">
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="0" t="n">
         <v>362</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="0" t="n">
         <v>1.08</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0" t="n">
         <v>0.34</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0" t="n">
         <v>463</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="0" t="n">
         <v>205</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="0" t="n">
         <v>378</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="0" t="n">
         <v>0.82</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0" t="n">
         <v>440</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0" t="n">
         <v>0.38</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0" t="n">
         <v>461</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="0" t="n">
         <v>247</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="0" t="n">
         <v>384</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="0" t="n">
         <v>0.7</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0" t="n">
         <v>437</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="0" t="n">
         <v>0.23</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0" t="n">
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="0" t="n">
         <v>248</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="0" t="n">
         <v>385</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="0" t="n">
         <v>0.26</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0" t="n">
         <v>405</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="0" t="n">
         <v>0.79</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0" t="n">
         <v>449</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="0" t="n">
         <v>671</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="0" t="n">
         <v>353</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="0" t="n">
         <v>0.68</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0" t="n">
         <v>405</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="0" t="n">
         <v>0.79</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0" t="n">
         <v>449</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="0" t="n">
         <v>682</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="0" t="n">
         <v>354</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="0" t="n">
         <v>0.66</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0" t="n">
         <v>404</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="0" t="n">
         <v>0.41</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0" t="n">
         <v>427</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="0" t="n">
         <v>727</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="0" t="n">
         <v>353</v>
       </c>
-      <c r="E21">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="F21">
+      <c r="E21" s="0" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="F21" s="0" t="n">
         <v>440</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="0" t="n">
         <v>0.48</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0" t="n">
         <v>467</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="0" t="n">
         <v>731</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="0" t="n">
         <v>382</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="0" t="n">
         <v>0.53</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0" t="n">
         <v>422</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="0" t="n">
         <v>0.61</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0" t="n">
         <v>456</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="0" t="n">
         <v>734</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="0" t="n">
         <v>372</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="0" t="n">
         <v>0.82</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0" t="n">
         <v>434</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="0" t="n">
         <v>0.43</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0" t="n">
         <v>458</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="0" t="n">
         <v>748</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="0" t="n">
         <v>386</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="0" t="n">
         <v>0.59</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="0" t="n">
         <v>431</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="0" t="n">
         <v>0.32</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="0" t="n">
         <v>449</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="0" t="n">
         <v>199</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="0" t="n">
         <v>343</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="0" t="n">
         <v>1.24</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="0" t="n">
         <v>437</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="0" t="n">
         <v>0.52</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="0" t="n">
         <v>466</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="0" t="n">
         <v>244</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="0" t="n">
         <v>360</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="0" t="n">
         <v>452</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="0" t="n">
         <v>217</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="0" t="n">
         <v>386</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="0" t="n">
         <v>467</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="0" t="n">
         <v>271</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="0" t="n">
         <v>1.19</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="0" t="n">
         <v>438</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="0" t="n">
         <v>348</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="0" t="n">
         <v>1.24</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="0" t="n">
         <v>442</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="0" t="n">
         <v>144</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="0" t="n">
         <v>356</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="0" t="n">
         <v>428</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>